<commit_message>
Opdater listbox på sensoroverblik.
</commit_message>
<xml_diff>
--- a/BemaerkningsFil.xlsx
+++ b/BemaerkningsFil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Documents\Sundhedsteknologi\7. Semester\Bachelor\MatLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8888260E-59E3-4767-8113-0249EFE7A581}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5E3F27A-9152-466C-84C7-EE4DEF47E0ED}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="8400" xr2:uid="{B3D96487-A2FC-4D60-BBCF-B4AC53D08ADA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="11">
   <si>
     <t>Teknologi</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>Borger kræver to personaler</t>
+  </si>
+  <si>
+    <t>Sensor2</t>
+  </si>
+  <si>
+    <t>CarendoSensor</t>
+  </si>
+  <si>
+    <t>Sensor1</t>
   </si>
 </sst>
 </file>
@@ -404,15 +413,16 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -536,7 +546,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="1">
-        <v>43382.739583333336</v>
+        <v>43380.823182870372</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -547,10 +557,10 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1">
-        <v>43380.823182870372</v>
+        <v>43381.313101851854</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
@@ -561,10 +571,10 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1">
-        <v>43380.823182870372</v>
+        <v>43381.313101851854</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
@@ -572,16 +582,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1">
-        <v>43382.739583333336</v>
+        <v>43380.620393518519</v>
       </c>
       <c r="D12" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ændringer i GUI'er. Tilføj bemærkning virker.
</commit_message>
<xml_diff>
--- a/BemaerkningsFil.xlsx
+++ b/BemaerkningsFil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruger\Documents\Sundhedsteknologi\7. Semester\Bachelor\MatLab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5E3F27A-9152-466C-84C7-EE4DEF47E0ED}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B1D19B1-F34D-4040-89C2-81F6F24CD250}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11496" windowHeight="8400" xr2:uid="{B3D96487-A2FC-4D60-BBCF-B4AC53D08ADA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="13">
   <si>
     <t>Teknologi</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>Sensor1</t>
+  </si>
+  <si>
+    <t>Andet: Urolig borger</t>
+  </si>
+  <si>
+    <t>Sensor3</t>
   </si>
 </sst>
 </file>
@@ -410,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C53ABE-08A2-4609-8B8D-CD8A29661281}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
@@ -418,11 +424,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -594,6 +599,76 @@
         <v>7</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1">
+        <v>43381.313101851854</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1">
+        <v>43380.862523148149</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1">
+        <v>43381.322974537034</v>
+      </c>
+      <c r="D15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1">
+        <v>43381.322974537034</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1">
+        <v>43381.313101851854</v>
+      </c>
+      <c r="D17" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Overskuelig kode for overblikskærmen
</commit_message>
<xml_diff>
--- a/BemaerkningsFil.xlsx
+++ b/BemaerkningsFil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruger\Documents\Bachelorprojekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{09EB449B-1FBE-49A9-B9AE-25BADBBC3ADA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{385933C3-B3B1-4B5B-A29D-2DD5AC473EE8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11500" windowHeight="8400" xr2:uid="{B3D96487-A2FC-4D60-BBCF-B4AC53D08ADA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="14">
   <si>
     <t>Teknologi</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Sensor3</t>
+  </si>
+  <si>
+    <t>Btw.</t>
   </si>
 </sst>
 </file>
@@ -416,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C53ABE-08A2-4609-8B8D-CD8A29661281}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -487,6 +490,9 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -532,16 +538,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C8" s="1">
-        <v>43381.313101851854</v>
+        <v>43380.620393518519</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
@@ -552,21 +558,21 @@
         <v>10</v>
       </c>
       <c r="C9" s="1">
-        <v>43380.620393518519</v>
+        <v>43380.862523148149</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C10" s="1">
-        <v>43381.313101851854</v>
+        <v>43381.322974537034</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
@@ -580,51 +586,9 @@
         <v>10</v>
       </c>
       <c r="C11" s="1">
-        <v>43380.862523148149</v>
+        <v>43383.646249999998</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="1">
-        <v>43381.322974537034</v>
-      </c>
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1">
-        <v>43381.313101851854</v>
-      </c>
-      <c r="D13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="1">
-        <v>43383.646249999998</v>
-      </c>
-      <c r="D14" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Jeg har bare klikket rundt, og ikke foretaget ændringer bevidst
</commit_message>
<xml_diff>
--- a/BemaerkningsFil.xlsx
+++ b/BemaerkningsFil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruger\Documents\Bachelorprojekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{398BCEA8-E8AE-4005-AE0D-0EACD986727E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6EEE2DC-4B16-4E26-8E92-02E8D289330D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11500" windowHeight="8400" xr2:uid="{B3D96487-A2FC-4D60-BBCF-B4AC53D08ADA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="15">
   <si>
     <t>Teknologi</t>
   </si>
@@ -422,7 +422,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C53ABE-08A2-4609-8B8D-CD8A29661281}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
@@ -791,6 +791,20 @@
         <v>4</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="1">
+        <v>43482.496817129628</v>
+      </c>
+      <c r="D26" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>